<commit_message>
added 2021 bar data, updated directory structure naming
</commit_message>
<xml_diff>
--- a/data/field_observations/groundwater/well_missing_data.xlsx
+++ b/data/field_observations/groundwater/well_missing_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/field_observations/groundwater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC83B459-29AB-8E4B-B74D-DD2C9CCC5F4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471D7B90-1A28-324C-81C4-7B1AACA81EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23360" yWindow="460" windowWidth="10240" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>